<commit_message>
plantillas financiera y tecnologicas
</commit_message>
<xml_diff>
--- a/Platillas de Valoracion/Primeras Valoraciones/Tecnologico/PLANTILLA DE VALORACIÓN 2021- ss&c.xlsx
+++ b/Platillas de Valoracion/Primeras Valoraciones/Tecnologico/PLANTILLA DE VALORACIÓN 2021- ss&c.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10411"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A273ACF3-FAF2-407C-8D56-1008107363B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E4A30D-E3B7-5341-BE83-9973ECB6E693}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1.Income statement" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="B15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
@@ -45,7 +45,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Autor:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -69,7 +69,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Autor:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -93,7 +93,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Autor:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -117,7 +117,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Autor:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -152,7 +152,7 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
@@ -165,7 +165,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Autor:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -186,7 +186,7 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="B15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
@@ -199,7 +199,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Autor:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -223,7 +223,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Autor:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -244,7 +244,7 @@
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
@@ -257,7 +257,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Autor:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -282,7 +282,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Autor:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -306,7 +306,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Autor:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -330,7 +330,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Autor:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -683,11 +683,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="#,##0.0;[Red]\-#,##0.0"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="0.0%"/>
-    <numFmt numFmtId="167" formatCode="_-[$$-2809]* #,##0_-;\-[$$-2809]* #,##0_-;_-[$$-2809]* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0;[Red]\-#,##0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
+    <numFmt numFmtId="168" formatCode="_-[$$-2809]* #,##0_-;\-[$$-2809]* #,##0_-;_-[$$-2809]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="29" x14ac:knownFonts="1">
     <font>
@@ -1390,7 +1390,7 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="316">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1434,7 +1434,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1540,22 +1540,22 @@
     <xf numFmtId="1" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="19" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1624,10 +1624,10 @@
     <xf numFmtId="2" fontId="17" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="15" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="23" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1760,13 +1760,13 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1781,31 +1781,31 @@
     <xf numFmtId="2" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1820,7 +1820,7 @@
     <xf numFmtId="1" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1912,10 +1912,10 @@
     <xf numFmtId="9" fontId="23" fillId="4" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="5" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="17" fillId="5" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="38" fontId="17" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1939,7 +1939,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="40" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1954,7 +1954,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="15" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="19" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2028,19 +2028,19 @@
     <xf numFmtId="38" fontId="17" fillId="5" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="23" fillId="4" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="23" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="23" fillId="4" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="23" fillId="4" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="23" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="23" fillId="4" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="38" fontId="17" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="38" fontId="17" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2058,13 +2058,13 @@
     <xf numFmtId="38" fontId="17" fillId="5" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="17" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2073,28 +2073,28 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="13" fillId="4" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="13" fillId="4" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="13" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="13" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="13" fillId="4" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="13" fillId="4" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="13" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="13" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="13" fillId="4" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="13" fillId="4" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="13" fillId="4" borderId="39" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="13" fillId="4" borderId="39" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="13" fillId="4" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="13" fillId="4" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="13" fillId="4" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="13" fillId="4" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2103,7 +2103,7 @@
     <xf numFmtId="9" fontId="23" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="17" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2133,7 +2133,7 @@
     <xf numFmtId="40" fontId="15" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="38" fontId="17" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2151,13 +2151,13 @@
     <xf numFmtId="2" fontId="4" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="40" fontId="0" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="16" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2235,6 +2235,42 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2244,48 +2280,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2303,9 +2303,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Moneda" xfId="2" builtinId="4"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -2323,7 +2323,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2780,7 +2780,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3102,21 +3102,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:S46"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="40" customWidth="1"/>
-    <col min="2" max="2" width="42.28515625" style="31" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" style="40" customWidth="1"/>
+    <col min="2" max="2" width="42.33203125" style="31" customWidth="1"/>
     <col min="3" max="14" width="11" style="71" customWidth="1"/>
-    <col min="15" max="15" width="14.5703125" style="40" customWidth="1"/>
-    <col min="16" max="16384" width="11.42578125" style="40"/>
+    <col min="15" max="15" width="14.5" style="40" customWidth="1"/>
+    <col min="16" max="16384" width="11.5" style="40"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="271"/>
       <c r="C2" s="274"/>
       <c r="D2" s="275"/>
@@ -3135,7 +3135,7 @@
       <c r="Q2" s="14"/>
       <c r="R2" s="14"/>
     </row>
-    <row r="3" spans="2:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="272"/>
       <c r="C3" s="277"/>
       <c r="D3" s="278"/>
@@ -3154,7 +3154,7 @@
       <c r="Q3" s="14"/>
       <c r="R3" s="14"/>
     </row>
-    <row r="4" spans="2:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="272"/>
       <c r="C4" s="277"/>
       <c r="D4" s="278"/>
@@ -3173,7 +3173,7 @@
       <c r="Q4" s="14"/>
       <c r="R4" s="14"/>
     </row>
-    <row r="5" spans="2:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="272"/>
       <c r="C5" s="277"/>
       <c r="D5" s="278"/>
@@ -3192,7 +3192,7 @@
       <c r="Q5" s="14"/>
       <c r="R5" s="14"/>
     </row>
-    <row r="6" spans="2:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="272"/>
       <c r="C6" s="277"/>
       <c r="D6" s="278"/>
@@ -3210,7 +3210,7 @@
       <c r="P6" s="24"/>
       <c r="Q6" s="14"/>
     </row>
-    <row r="7" spans="2:19" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:19" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="272"/>
       <c r="C7" s="280"/>
       <c r="D7" s="281"/>
@@ -3228,7 +3228,7 @@
       <c r="P7" s="24"/>
       <c r="Q7" s="14"/>
     </row>
-    <row r="8" spans="2:19" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:19" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="273"/>
       <c r="C8" s="32">
         <v>2014</v>
@@ -3270,7 +3270,7 @@
       <c r="P8" s="14"/>
       <c r="Q8" s="14"/>
     </row>
-    <row r="9" spans="2:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="67" t="s">
         <v>36</v>
       </c>
@@ -3290,7 +3290,7 @@
       <c r="P9" s="14"/>
       <c r="Q9" s="14"/>
     </row>
-    <row r="10" spans="2:19" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:19" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="62" t="s">
         <v>15</v>
       </c>
@@ -3339,7 +3339,7 @@
       <c r="P10" s="14"/>
       <c r="Q10" s="14"/>
     </row>
-    <row r="11" spans="2:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="198" t="s">
         <v>35</v>
       </c>
@@ -3400,7 +3400,7 @@
       <c r="Q11" s="14"/>
       <c r="S11"/>
     </row>
-    <row r="12" spans="2:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="200" t="s">
         <v>6</v>
       </c>
@@ -3456,7 +3456,7 @@
       <c r="P12" s="18"/>
       <c r="Q12" s="14"/>
     </row>
-    <row r="13" spans="2:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="198" t="s">
         <v>16</v>
       </c>
@@ -3512,7 +3512,7 @@
       <c r="P13" s="14"/>
       <c r="Q13" s="14"/>
     </row>
-    <row r="14" spans="2:19" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:19" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="197" t="s">
         <v>0</v>
       </c>
@@ -3561,7 +3561,7 @@
       <c r="P14" s="14"/>
       <c r="Q14" s="14"/>
     </row>
-    <row r="15" spans="2:19" ht="15.95" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:19" ht="16" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="62" t="s">
         <v>7</v>
       </c>
@@ -3610,7 +3610,7 @@
       <c r="P15" s="14"/>
       <c r="Q15" s="14"/>
     </row>
-    <row r="16" spans="2:19" ht="15.95" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:19" ht="16" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="198" t="s">
         <v>17</v>
       </c>
@@ -3670,7 +3670,7 @@
       </c>
       <c r="Q16" s="14"/>
     </row>
-    <row r="17" spans="2:17" ht="15.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17" ht="16" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B17" s="283" t="s">
         <v>55</v>
       </c>
@@ -3714,7 +3714,7 @@
       <c r="P17" s="14"/>
       <c r="Q17" s="14"/>
     </row>
-    <row r="18" spans="2:17" ht="15.95" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:17" ht="16" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="284"/>
       <c r="C18" s="251"/>
       <c r="D18" s="251"/>
@@ -3732,7 +3732,7 @@
       <c r="P18" s="14"/>
       <c r="Q18" s="14"/>
     </row>
-    <row r="19" spans="2:17" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:17" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="196" t="s">
         <v>1</v>
       </c>
@@ -3788,7 +3788,7 @@
       <c r="P19" s="14"/>
       <c r="Q19" s="14"/>
     </row>
-    <row r="20" spans="2:17" ht="15.95" customHeight="1" collapsed="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:17" ht="16" customHeight="1" collapsed="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="197" t="s">
         <v>2</v>
       </c>
@@ -3837,7 +3837,7 @@
       <c r="P20" s="14"/>
       <c r="Q20" s="14"/>
     </row>
-    <row r="21" spans="2:17" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:17" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B21" s="198" t="s">
         <v>10</v>
       </c>
@@ -3897,7 +3897,7 @@
       </c>
       <c r="Q21" s="14"/>
     </row>
-    <row r="22" spans="2:17" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:17" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="199" t="s">
         <v>3</v>
       </c>
@@ -3953,7 +3953,7 @@
       <c r="P22" s="14"/>
       <c r="Q22" s="14"/>
     </row>
-    <row r="23" spans="2:17" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:17" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="197" t="s">
         <v>4</v>
       </c>
@@ -4002,7 +4002,7 @@
       <c r="P23" s="14"/>
       <c r="Q23" s="14"/>
     </row>
-    <row r="24" spans="2:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="200" t="s">
         <v>5</v>
       </c>
@@ -4058,7 +4058,7 @@
       <c r="P24" s="14"/>
       <c r="Q24" s="14"/>
     </row>
-    <row r="25" spans="2:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="198" t="s">
         <v>37</v>
       </c>
@@ -4114,7 +4114,7 @@
       <c r="P25" s="14"/>
       <c r="Q25" s="14"/>
     </row>
-    <row r="26" spans="2:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="62" t="s">
         <v>18</v>
       </c>
@@ -4170,7 +4170,7 @@
       <c r="P26" s="14"/>
       <c r="Q26" s="14"/>
     </row>
-    <row r="27" spans="2:17" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:17" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="68" t="s">
         <v>56</v>
       </c>
@@ -4212,9 +4212,11 @@
       </c>
       <c r="O27" s="203"/>
       <c r="P27" s="14"/>
-      <c r="Q27" s="14"/>
-    </row>
-    <row r="28" spans="2:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q27" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="69"/>
       <c r="C28" s="81"/>
       <c r="D28" s="81"/>
@@ -4232,7 +4234,7 @@
       <c r="P28" s="14"/>
       <c r="Q28" s="14"/>
     </row>
-    <row r="29" spans="2:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="69"/>
       <c r="C29" s="82"/>
       <c r="D29" s="82"/>
@@ -4250,7 +4252,7 @@
       <c r="P29" s="14"/>
       <c r="Q29" s="14"/>
     </row>
-    <row r="30" spans="2:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="69"/>
       <c r="C30" s="81"/>
       <c r="D30" s="81"/>
@@ -4268,7 +4270,7 @@
       <c r="P30" s="14"/>
       <c r="Q30" s="14"/>
     </row>
-    <row r="31" spans="2:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="269"/>
       <c r="C31" s="269"/>
       <c r="D31" s="269"/>
@@ -4286,7 +4288,7 @@
       <c r="P31" s="14"/>
       <c r="Q31" s="14"/>
     </row>
-    <row r="32" spans="2:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="69"/>
       <c r="C32" s="81"/>
       <c r="D32" s="81"/>
@@ -4301,7 +4303,7 @@
       <c r="M32" s="100"/>
       <c r="N32" s="99"/>
     </row>
-    <row r="33" spans="2:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="69"/>
       <c r="C33" s="76"/>
       <c r="D33" s="76"/>
@@ -4316,7 +4318,7 @@
       <c r="M33" s="100"/>
       <c r="N33" s="99"/>
     </row>
-    <row r="34" spans="2:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="70"/>
       <c r="C34" s="95"/>
       <c r="D34" s="95"/>
@@ -4331,7 +4333,7 @@
       <c r="M34" s="100"/>
       <c r="N34" s="99"/>
     </row>
-    <row r="35" spans="2:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="69"/>
       <c r="C35" s="81"/>
       <c r="D35" s="81"/>
@@ -4346,7 +4348,7 @@
       <c r="M35" s="100"/>
       <c r="N35" s="99"/>
     </row>
-    <row r="36" spans="2:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="69"/>
       <c r="C36" s="81"/>
       <c r="D36" s="82"/>
@@ -4361,7 +4363,7 @@
       <c r="M36" s="100"/>
       <c r="N36" s="99"/>
     </row>
-    <row r="37" spans="2:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="70"/>
       <c r="C37" s="95"/>
       <c r="D37" s="95"/>
@@ -4376,7 +4378,7 @@
       <c r="M37" s="100"/>
       <c r="N37" s="99"/>
     </row>
-    <row r="38" spans="2:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="69"/>
       <c r="C38" s="81"/>
       <c r="D38" s="81"/>
@@ -4391,7 +4393,7 @@
       <c r="M38" s="100"/>
       <c r="N38" s="99"/>
     </row>
-    <row r="39" spans="2:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="69"/>
       <c r="C39" s="82"/>
       <c r="D39" s="81"/>
@@ -4406,7 +4408,7 @@
       <c r="M39" s="100"/>
       <c r="N39" s="99"/>
     </row>
-    <row r="40" spans="2:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="69"/>
       <c r="C40" s="81"/>
       <c r="D40" s="81"/>
@@ -4421,7 +4423,7 @@
       <c r="M40" s="100"/>
       <c r="N40" s="99"/>
     </row>
-    <row r="41" spans="2:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="69"/>
       <c r="C41" s="82"/>
       <c r="D41" s="82"/>
@@ -4436,7 +4438,7 @@
       <c r="M41" s="100"/>
       <c r="N41" s="99"/>
     </row>
-    <row r="42" spans="2:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="70"/>
       <c r="C42" s="95"/>
       <c r="D42" s="95"/>
@@ -4451,7 +4453,7 @@
       <c r="M42" s="100"/>
       <c r="N42" s="99"/>
     </row>
-    <row r="43" spans="2:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="270"/>
       <c r="C43" s="270"/>
       <c r="D43" s="270"/>
@@ -4466,7 +4468,7 @@
       <c r="M43" s="99"/>
       <c r="N43" s="99"/>
     </row>
-    <row r="44" spans="2:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="69"/>
       <c r="C44" s="81"/>
       <c r="D44" s="81"/>
@@ -4481,7 +4483,7 @@
       <c r="M44" s="99"/>
       <c r="N44" s="99"/>
     </row>
-    <row r="45" spans="2:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="69"/>
       <c r="C45" s="81"/>
       <c r="D45" s="81"/>
@@ -4496,7 +4498,7 @@
       <c r="M45" s="99"/>
       <c r="N45" s="99"/>
     </row>
-    <row r="46" spans="2:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="69"/>
       <c r="C46" s="81"/>
       <c r="D46" s="81"/>
@@ -4534,17 +4536,17 @@
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" customWidth="1"/>
-    <col min="2" max="2" width="46.42578125" style="29" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5" customWidth="1"/>
+    <col min="2" max="2" width="46.5" style="29" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="14" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="271"/>
       <c r="C2" s="286"/>
       <c r="D2" s="287"/>
@@ -4559,7 +4561,7 @@
       <c r="M2" s="287"/>
       <c r="N2" s="288"/>
     </row>
-    <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="272"/>
       <c r="C3" s="289"/>
       <c r="D3" s="290"/>
@@ -4574,7 +4576,7 @@
       <c r="M3" s="290"/>
       <c r="N3" s="291"/>
     </row>
-    <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="272"/>
       <c r="C4" s="289"/>
       <c r="D4" s="290"/>
@@ -4589,7 +4591,7 @@
       <c r="M4" s="290"/>
       <c r="N4" s="291"/>
     </row>
-    <row r="5" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="272"/>
       <c r="C5" s="289"/>
       <c r="D5" s="290"/>
@@ -4604,7 +4606,7 @@
       <c r="M5" s="290"/>
       <c r="N5" s="291"/>
     </row>
-    <row r="6" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="272"/>
       <c r="C6" s="289"/>
       <c r="D6" s="290"/>
@@ -4619,7 +4621,7 @@
       <c r="M6" s="290"/>
       <c r="N6" s="291"/>
     </row>
-    <row r="7" spans="2:15" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="272"/>
       <c r="C7" s="289"/>
       <c r="D7" s="290"/>
@@ -4634,7 +4636,7 @@
       <c r="M7" s="290"/>
       <c r="N7" s="291"/>
     </row>
-    <row r="8" spans="2:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="285"/>
       <c r="C8" s="33">
         <v>2014</v>
@@ -4673,7 +4675,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B9" s="61" t="s">
         <v>38</v>
       </c>
@@ -4690,7 +4692,7 @@
       <c r="M9" s="36"/>
       <c r="N9" s="37"/>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B10" s="62" t="s">
         <v>6</v>
       </c>
@@ -4743,7 +4745,7 @@
         <v>2194.2853647749998</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B11" s="185" t="s">
         <v>40</v>
       </c>
@@ -4790,7 +4792,7 @@
         <v>135.79635825000003</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B12" s="186" t="s">
         <v>39</v>
       </c>
@@ -4843,7 +4845,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B13" s="186" t="s">
         <v>41</v>
       </c>
@@ -4896,7 +4898,7 @@
         <v>244.22265801749995</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B14" s="187" t="s">
         <v>80</v>
       </c>
@@ -4949,7 +4951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B15" s="63" t="s">
         <v>8</v>
       </c>
@@ -5003,7 +5005,7 @@
       </c>
       <c r="O15" s="214"/>
     </row>
-    <row r="16" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="64" t="s">
         <v>9</v>
       </c>
@@ -5057,7 +5059,7 @@
       </c>
       <c r="O16" s="204"/>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B17" s="28"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -5072,7 +5074,7 @@
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B18" s="4"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -5087,7 +5089,7 @@
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B19" s="28"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -5102,7 +5104,7 @@
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B20" s="28"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -5117,7 +5119,7 @@
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B21" s="28"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -5132,7 +5134,7 @@
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B22" s="28"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -5147,7 +5149,7 @@
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B23" s="28"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -5162,7 +5164,7 @@
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B24" s="28"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -5177,7 +5179,7 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B25" s="27"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -5192,7 +5194,7 @@
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B26" s="27"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -5207,7 +5209,7 @@
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B27" s="27"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -5222,7 +5224,7 @@
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B28" s="27"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -5237,7 +5239,7 @@
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B29" s="27"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -5252,7 +5254,7 @@
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B30" s="27"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -5287,17 +5289,17 @@
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.140625" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="4.1640625" customWidth="1"/>
+    <col min="2" max="2" width="45.6640625" customWidth="1"/>
+    <col min="3" max="3" width="8.5" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="15" max="15" width="13.85546875" customWidth="1"/>
+    <col min="15" max="15" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="292"/>
       <c r="C2" s="286"/>
       <c r="D2" s="287"/>
@@ -5312,7 +5314,7 @@
       <c r="M2" s="287"/>
       <c r="N2" s="288"/>
     </row>
-    <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="293"/>
       <c r="C3" s="289"/>
       <c r="D3" s="290"/>
@@ -5327,7 +5329,7 @@
       <c r="M3" s="290"/>
       <c r="N3" s="291"/>
     </row>
-    <row r="4" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="293"/>
       <c r="C4" s="289"/>
       <c r="D4" s="290"/>
@@ -5342,7 +5344,7 @@
       <c r="M4" s="290"/>
       <c r="N4" s="291"/>
     </row>
-    <row r="5" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="293"/>
       <c r="C5" s="289"/>
       <c r="D5" s="290"/>
@@ -5357,7 +5359,7 @@
       <c r="M5" s="290"/>
       <c r="N5" s="291"/>
     </row>
-    <row r="6" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="293"/>
       <c r="C6" s="289"/>
       <c r="D6" s="290"/>
@@ -5372,7 +5374,7 @@
       <c r="M6" s="290"/>
       <c r="N6" s="291"/>
     </row>
-    <row r="7" spans="2:16" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:16" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="293"/>
       <c r="C7" s="289"/>
       <c r="D7" s="290"/>
@@ -5387,7 +5389,7 @@
       <c r="M7" s="290"/>
       <c r="N7" s="291"/>
     </row>
-    <row r="8" spans="2:16" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:16" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="293"/>
       <c r="C8" s="33">
         <v>2014</v>
@@ -5426,7 +5428,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="9" spans="2:16" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="42" t="s">
         <v>42</v>
       </c>
@@ -5443,7 +5445,7 @@
       <c r="M9" s="48"/>
       <c r="N9" s="49"/>
     </row>
-    <row r="10" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="205" t="s">
         <v>11</v>
       </c>
@@ -5503,7 +5505,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="11" spans="2:16" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B11" s="206" t="s">
         <v>43</v>
       </c>
@@ -5556,7 +5558,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B12" s="207" t="s">
         <v>41</v>
       </c>
@@ -5609,7 +5611,7 @@
         <v>244.22265801749995</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B13" s="208" t="s">
         <v>12</v>
       </c>
@@ -5662,7 +5664,7 @@
         <v>976.89063206999981</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B14" s="209" t="s">
         <v>47</v>
       </c>
@@ -5709,7 +5711,7 @@
       </c>
       <c r="O14" s="214"/>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B15" s="210" t="s">
         <v>44</v>
       </c>
@@ -5755,7 +5757,7 @@
         <v>8152.8866212499997</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B16" s="209" t="s">
         <v>45</v>
       </c>
@@ -5801,7 +5803,7 @@
         <v>10309.802461875001</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B17" s="209" t="s">
         <v>46</v>
       </c>
@@ -5847,7 +5849,7 @@
         <v>7295.2254112500004</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B18" s="211" t="s">
         <v>51</v>
       </c>
@@ -5900,7 +5902,7 @@
         <v>15181.369185937501</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B19" s="212" t="s">
         <v>52</v>
       </c>
@@ -5953,7 +5955,7 @@
         <v>4871.5667240624989</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B20" s="210"/>
       <c r="C20" s="58"/>
       <c r="D20" s="58"/>
@@ -5967,7 +5969,7 @@
       <c r="M20" s="59"/>
       <c r="N20" s="60"/>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B21" s="209" t="s">
         <v>48</v>
       </c>
@@ -6020,7 +6022,7 @@
         <v>0.13390821763554178</v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B22" s="209" t="s">
         <v>54</v>
       </c>
@@ -6073,7 +6075,7 @@
         <v>0.25681949174744567</v>
       </c>
     </row>
-    <row r="23" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="213" t="s">
         <v>53</v>
       </c>
@@ -6126,7 +6128,7 @@
         <v>8.2411097099621661E-2</v>
       </c>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -6141,7 +6143,7 @@
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -6156,7 +6158,7 @@
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -6171,7 +6173,7 @@
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -6186,7 +6188,7 @@
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -6217,39 +6219,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:V41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="T18" sqref="T18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="35.5703125" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" customWidth="1"/>
-    <col min="13" max="14" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="35.5" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
+    <col min="10" max="10" width="10.5" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="15.5" customWidth="1"/>
+    <col min="13" max="14" width="10.5" customWidth="1"/>
     <col min="15" max="15" width="7" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:22" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="292"/>
-      <c r="C2" s="301"/>
-      <c r="D2" s="302"/>
-      <c r="E2" s="302"/>
-      <c r="F2" s="302"/>
-      <c r="G2" s="302"/>
-      <c r="H2" s="302"/>
-      <c r="I2" s="302"/>
-      <c r="J2" s="302"/>
-      <c r="K2" s="302"/>
-      <c r="L2" s="302"/>
-      <c r="M2" s="302"/>
-      <c r="N2" s="303"/>
+      <c r="C2" s="295"/>
+      <c r="D2" s="296"/>
+      <c r="E2" s="296"/>
+      <c r="F2" s="296"/>
+      <c r="G2" s="296"/>
+      <c r="H2" s="296"/>
+      <c r="I2" s="296"/>
+      <c r="J2" s="296"/>
+      <c r="K2" s="296"/>
+      <c r="L2" s="296"/>
+      <c r="M2" s="296"/>
+      <c r="N2" s="297"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
@@ -6259,20 +6261,20 @@
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
     </row>
-    <row r="3" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="293"/>
-      <c r="C3" s="304"/>
-      <c r="D3" s="305"/>
-      <c r="E3" s="305"/>
-      <c r="F3" s="305"/>
-      <c r="G3" s="305"/>
-      <c r="H3" s="305"/>
-      <c r="I3" s="305"/>
-      <c r="J3" s="305"/>
-      <c r="K3" s="305"/>
-      <c r="L3" s="305"/>
-      <c r="M3" s="305"/>
-      <c r="N3" s="306"/>
+      <c r="C3" s="298"/>
+      <c r="D3" s="299"/>
+      <c r="E3" s="299"/>
+      <c r="F3" s="299"/>
+      <c r="G3" s="299"/>
+      <c r="H3" s="299"/>
+      <c r="I3" s="299"/>
+      <c r="J3" s="299"/>
+      <c r="K3" s="299"/>
+      <c r="L3" s="299"/>
+      <c r="M3" s="299"/>
+      <c r="N3" s="300"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
@@ -6282,20 +6284,20 @@
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
     </row>
-    <row r="4" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="293"/>
-      <c r="C4" s="304"/>
-      <c r="D4" s="305"/>
-      <c r="E4" s="305"/>
-      <c r="F4" s="305"/>
-      <c r="G4" s="305"/>
-      <c r="H4" s="305"/>
-      <c r="I4" s="305"/>
-      <c r="J4" s="305"/>
-      <c r="K4" s="305"/>
-      <c r="L4" s="305"/>
-      <c r="M4" s="305"/>
-      <c r="N4" s="306"/>
+      <c r="C4" s="298"/>
+      <c r="D4" s="299"/>
+      <c r="E4" s="299"/>
+      <c r="F4" s="299"/>
+      <c r="G4" s="299"/>
+      <c r="H4" s="299"/>
+      <c r="I4" s="299"/>
+      <c r="J4" s="299"/>
+      <c r="K4" s="299"/>
+      <c r="L4" s="299"/>
+      <c r="M4" s="299"/>
+      <c r="N4" s="300"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
@@ -6305,20 +6307,20 @@
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
     </row>
-    <row r="5" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="293"/>
-      <c r="C5" s="304"/>
-      <c r="D5" s="305"/>
-      <c r="E5" s="305"/>
-      <c r="F5" s="305"/>
-      <c r="G5" s="305"/>
-      <c r="H5" s="305"/>
-      <c r="I5" s="305"/>
-      <c r="J5" s="305"/>
-      <c r="K5" s="305"/>
-      <c r="L5" s="305"/>
-      <c r="M5" s="305"/>
-      <c r="N5" s="306"/>
+      <c r="C5" s="298"/>
+      <c r="D5" s="299"/>
+      <c r="E5" s="299"/>
+      <c r="F5" s="299"/>
+      <c r="G5" s="299"/>
+      <c r="H5" s="299"/>
+      <c r="I5" s="299"/>
+      <c r="J5" s="299"/>
+      <c r="K5" s="299"/>
+      <c r="L5" s="299"/>
+      <c r="M5" s="299"/>
+      <c r="N5" s="300"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
@@ -6328,20 +6330,20 @@
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
     </row>
-    <row r="6" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="293"/>
-      <c r="C6" s="304"/>
-      <c r="D6" s="305"/>
-      <c r="E6" s="305"/>
-      <c r="F6" s="305"/>
-      <c r="G6" s="305"/>
-      <c r="H6" s="305"/>
-      <c r="I6" s="305"/>
-      <c r="J6" s="305"/>
-      <c r="K6" s="305"/>
-      <c r="L6" s="305"/>
-      <c r="M6" s="305"/>
-      <c r="N6" s="306"/>
+      <c r="C6" s="298"/>
+      <c r="D6" s="299"/>
+      <c r="E6" s="299"/>
+      <c r="F6" s="299"/>
+      <c r="G6" s="299"/>
+      <c r="H6" s="299"/>
+      <c r="I6" s="299"/>
+      <c r="J6" s="299"/>
+      <c r="K6" s="299"/>
+      <c r="L6" s="299"/>
+      <c r="M6" s="299"/>
+      <c r="N6" s="300"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
@@ -6351,20 +6353,20 @@
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
     </row>
-    <row r="7" spans="2:22" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:22" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="293"/>
-      <c r="C7" s="304"/>
-      <c r="D7" s="305"/>
-      <c r="E7" s="305"/>
-      <c r="F7" s="305"/>
-      <c r="G7" s="305"/>
-      <c r="H7" s="305"/>
-      <c r="I7" s="305"/>
-      <c r="J7" s="307"/>
-      <c r="K7" s="307"/>
-      <c r="L7" s="307"/>
-      <c r="M7" s="307"/>
-      <c r="N7" s="308"/>
+      <c r="C7" s="298"/>
+      <c r="D7" s="299"/>
+      <c r="E7" s="299"/>
+      <c r="F7" s="299"/>
+      <c r="G7" s="299"/>
+      <c r="H7" s="299"/>
+      <c r="I7" s="299"/>
+      <c r="J7" s="301"/>
+      <c r="K7" s="301"/>
+      <c r="L7" s="301"/>
+      <c r="M7" s="301"/>
+      <c r="N7" s="302"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
@@ -6374,7 +6376,7 @@
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
     </row>
-    <row r="8" spans="2:22" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:22" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="293"/>
       <c r="C8" s="33">
         <v>2014</v>
@@ -6421,7 +6423,7 @@
       <c r="U8" s="1"/>
       <c r="V8" s="1"/>
     </row>
-    <row r="9" spans="2:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="114" t="s">
         <v>27</v>
       </c>
@@ -6437,10 +6439,10 @@
       <c r="L9" s="30"/>
       <c r="M9" s="58"/>
       <c r="N9" s="118"/>
-      <c r="O9" s="294" t="s">
+      <c r="O9" s="306" t="s">
         <v>14</v>
       </c>
-      <c r="P9" s="295"/>
+      <c r="P9" s="307"/>
       <c r="Q9" s="15">
         <v>72</v>
       </c>
@@ -6450,7 +6452,7 @@
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
     </row>
-    <row r="10" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:22" ht="16" x14ac:dyDescent="0.2">
       <c r="B10" s="62" t="s">
         <v>26</v>
       </c>
@@ -6493,7 +6495,7 @@
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
     </row>
-    <row r="11" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:22" ht="16" x14ac:dyDescent="0.2">
       <c r="B11" s="62" t="s">
         <v>60</v>
       </c>
@@ -6540,8 +6542,8 @@
       <c r="N11" s="218">
         <v>1000</v>
       </c>
-      <c r="O11" s="296"/>
-      <c r="P11" s="296"/>
+      <c r="O11" s="308"/>
+      <c r="P11" s="308"/>
       <c r="Q11" s="14"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
@@ -6549,7 +6551,7 @@
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
     </row>
-    <row r="12" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:22" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="110" t="s">
         <v>81</v>
       </c>
@@ -6601,8 +6603,8 @@
         <f>N11/'1.Income statement'!N12</f>
         <v>0.45572923925623465</v>
       </c>
-      <c r="O12" s="297"/>
-      <c r="P12" s="297"/>
+      <c r="O12" s="304"/>
+      <c r="P12" s="304"/>
       <c r="Q12" s="14"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
@@ -6610,7 +6612,7 @@
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
     </row>
-    <row r="13" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:22" ht="16" x14ac:dyDescent="0.2">
       <c r="B13" s="110" t="s">
         <v>82</v>
       </c>
@@ -6671,7 +6673,7 @@
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
     </row>
-    <row r="14" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:22" ht="16" x14ac:dyDescent="0.2">
       <c r="B14" s="111" t="s">
         <v>25</v>
       </c>
@@ -6705,8 +6707,8 @@
         <f t="shared" si="0"/>
         <v>20152</v>
       </c>
-      <c r="O14" s="309"/>
-      <c r="P14" s="309"/>
+      <c r="O14" s="303"/>
+      <c r="P14" s="303"/>
       <c r="Q14" s="14"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
@@ -6714,7 +6716,7 @@
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
     </row>
-    <row r="15" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:22" ht="16" x14ac:dyDescent="0.2">
       <c r="B15" s="62" t="s">
         <v>6</v>
       </c>
@@ -6766,8 +6768,8 @@
         <f>'1.Income statement'!N12</f>
         <v>2194.2853647749998</v>
       </c>
-      <c r="O15" s="297"/>
-      <c r="P15" s="297"/>
+      <c r="O15" s="304"/>
+      <c r="P15" s="304"/>
       <c r="Q15" s="14"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
@@ -6775,7 +6777,7 @@
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
     </row>
-    <row r="16" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:22" ht="16" x14ac:dyDescent="0.2">
       <c r="B16" s="62" t="s">
         <v>11</v>
       </c>
@@ -6827,8 +6829,8 @@
         <f>'1.Income statement'!N15</f>
         <v>1251.1132900874998</v>
       </c>
-      <c r="O16" s="297"/>
-      <c r="P16" s="297"/>
+      <c r="O16" s="304"/>
+      <c r="P16" s="304"/>
       <c r="Q16" s="14"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
@@ -6836,7 +6838,7 @@
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
     </row>
-    <row r="17" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:22" ht="16" x14ac:dyDescent="0.2">
       <c r="B17" s="62" t="s">
         <v>12</v>
       </c>
@@ -6888,8 +6890,8 @@
         <f>'1.Income statement'!N24</f>
         <v>976.89063206999981</v>
       </c>
-      <c r="O17" s="297"/>
-      <c r="P17" s="297"/>
+      <c r="O17" s="304"/>
+      <c r="P17" s="304"/>
       <c r="Q17" s="14"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
@@ -6897,7 +6899,7 @@
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
     </row>
-    <row r="18" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:22" ht="16" x14ac:dyDescent="0.2">
       <c r="B18" s="62" t="s">
         <v>13</v>
       </c>
@@ -6949,8 +6951,8 @@
         <f>'2.Flujos de caja'!N15</f>
         <v>1784.2663485074997</v>
       </c>
-      <c r="O18" s="297"/>
-      <c r="P18" s="297"/>
+      <c r="O18" s="304"/>
+      <c r="P18" s="304"/>
       <c r="Q18" s="5"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
@@ -6958,7 +6960,7 @@
       <c r="U18" s="1"/>
       <c r="V18" s="1"/>
     </row>
-    <row r="19" spans="2:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="62"/>
       <c r="C19" s="116"/>
       <c r="D19" s="107"/>
@@ -6981,7 +6983,7 @@
       <c r="U19" s="1"/>
       <c r="V19" s="1"/>
     </row>
-    <row r="20" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="126"/>
       <c r="C20" s="127" t="s">
         <v>49</v>
@@ -6999,8 +7001,8 @@
       <c r="L20" s="112"/>
       <c r="M20" s="112"/>
       <c r="N20" s="122"/>
-      <c r="O20" s="310"/>
-      <c r="P20" s="310"/>
+      <c r="O20" s="305"/>
+      <c r="P20" s="305"/>
       <c r="Q20" s="5"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
@@ -7008,7 +7010,7 @@
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
     </row>
-    <row r="21" spans="2:22" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:22" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B21" s="25" t="s">
         <v>21</v>
       </c>
@@ -7063,7 +7065,7 @@
       <c r="U21" s="1"/>
       <c r="V21" s="1"/>
     </row>
-    <row r="22" spans="2:22" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:22" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="25" t="s">
         <v>22</v>
       </c>
@@ -7105,10 +7107,10 @@
         <f>IF(N11&lt;0,N18*$Q$22-N11,IF(N11=0,N18*$Q$22,IF(N11&gt;0,N18*$Q$22)))/'1.Income statement'!N27</f>
         <v>134.15536454943609</v>
       </c>
-      <c r="O22" s="298" t="s">
+      <c r="O22" s="309" t="s">
         <v>29</v>
       </c>
-      <c r="P22" s="299"/>
+      <c r="P22" s="310"/>
       <c r="Q22" s="9">
         <v>20</v>
       </c>
@@ -7118,7 +7120,7 @@
       <c r="U22" s="1"/>
       <c r="V22" s="1"/>
     </row>
-    <row r="23" spans="2:22" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:22" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="25" t="s">
         <v>23</v>
       </c>
@@ -7160,10 +7162,10 @@
         <f>((N15*$Q$23)-N11)/'1.Income statement'!N27</f>
         <v>119.9784980136278</v>
       </c>
-      <c r="O23" s="300" t="s">
+      <c r="O23" s="294" t="s">
         <v>30</v>
       </c>
-      <c r="P23" s="300"/>
+      <c r="P23" s="294"/>
       <c r="Q23" s="9">
         <v>15</v>
       </c>
@@ -7173,7 +7175,7 @@
       <c r="U23" s="1"/>
       <c r="V23" s="1"/>
     </row>
-    <row r="24" spans="2:22" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:22" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="26" t="s">
         <v>24</v>
       </c>
@@ -7215,10 +7217,10 @@
         <f>((N16*$Q$24)-N11)/'1.Income statement'!N27</f>
         <v>90.309269931390958</v>
       </c>
-      <c r="O24" s="300" t="s">
+      <c r="O24" s="294" t="s">
         <v>31</v>
       </c>
-      <c r="P24" s="300"/>
+      <c r="P24" s="294"/>
       <c r="Q24" s="9">
         <v>20</v>
       </c>
@@ -7228,7 +7230,7 @@
       <c r="U24" s="1"/>
       <c r="V24" s="1"/>
     </row>
-    <row r="25" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:22" ht="16" x14ac:dyDescent="0.2">
       <c r="B25" s="4"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -7251,7 +7253,7 @@
       <c r="U25" s="1"/>
       <c r="V25" s="1"/>
     </row>
-    <row r="26" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B26" s="2"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -7274,7 +7276,7 @@
       <c r="U26" s="1"/>
       <c r="V26" s="1"/>
     </row>
-    <row r="27" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -7297,7 +7299,7 @@
       <c r="U27" s="1"/>
       <c r="V27" s="1"/>
     </row>
-    <row r="28" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -7320,7 +7322,7 @@
       <c r="U28" s="1"/>
       <c r="V28" s="1"/>
     </row>
-    <row r="29" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -7343,7 +7345,7 @@
       <c r="U29" s="1"/>
       <c r="V29" s="1"/>
     </row>
-    <row r="30" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -7366,7 +7368,7 @@
       <c r="U30" s="1"/>
       <c r="V30" s="1"/>
     </row>
-    <row r="31" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -7389,7 +7391,7 @@
       <c r="U31" s="1"/>
       <c r="V31" s="1"/>
     </row>
-    <row r="32" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -7412,7 +7414,7 @@
       <c r="U32" s="1"/>
       <c r="V32" s="1"/>
     </row>
-    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -7435,11 +7437,16 @@
       <c r="U33" s="1"/>
       <c r="V33" s="1"/>
     </row>
-    <row r="41" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:22" x14ac:dyDescent="0.2">
       <c r="Q41" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O22:P22"/>
     <mergeCell ref="O23:P23"/>
     <mergeCell ref="O24:P24"/>
     <mergeCell ref="C2:N7"/>
@@ -7449,11 +7456,6 @@
     <mergeCell ref="O17:P17"/>
     <mergeCell ref="O18:P18"/>
     <mergeCell ref="O20:P20"/>
-    <mergeCell ref="B2:B8"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="O22:P22"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q12:Q13" xr:uid="{00000000-0002-0000-0300-000000000000}">
@@ -7475,13 +7477,13 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="105.140625" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="105.1640625" customWidth="1"/>
+    <col min="9" max="9" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="167" t="s">
         <v>71</v>
       </c>
@@ -7491,7 +7493,7 @@
       <c r="F3" s="164"/>
       <c r="G3" s="164"/>
     </row>
-    <row r="4" spans="2:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="166" t="s">
         <v>59</v>
       </c>
@@ -7503,7 +7505,7 @@
       <c r="H4" s="161"/>
       <c r="I4" s="165"/>
     </row>
-    <row r="5" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="162"/>
       <c r="C5" s="161"/>
       <c r="D5" s="161"/>
@@ -7513,7 +7515,7 @@
       <c r="H5" s="161"/>
       <c r="I5" s="165"/>
     </row>
-    <row r="6" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="311" t="s">
         <v>72</v>
       </c>
@@ -7525,7 +7527,7 @@
       <c r="H6" s="311"/>
       <c r="I6" s="311"/>
     </row>
-    <row r="7" spans="2:9" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="153"/>
       <c r="C7" s="153"/>
       <c r="D7" s="153"/>
@@ -7535,7 +7537,7 @@
       <c r="H7" s="153"/>
       <c r="I7" s="153"/>
     </row>
-    <row r="8" spans="2:9" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="170" t="s">
         <v>73</v>
       </c>
@@ -7547,7 +7549,7 @@
       <c r="H8" s="153"/>
       <c r="I8" s="153"/>
     </row>
-    <row r="9" spans="2:9" s="150" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" s="150" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="158" t="s">
         <v>61</v>
       </c>
@@ -7559,7 +7561,7 @@
       <c r="H9" s="155"/>
       <c r="I9" s="155"/>
     </row>
-    <row r="10" spans="2:9" s="150" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" s="150" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="156" t="s">
         <v>66</v>
       </c>
@@ -7571,7 +7573,7 @@
       <c r="H10" s="155"/>
       <c r="I10" s="155"/>
     </row>
-    <row r="11" spans="2:9" s="150" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" s="150" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="156" t="s">
         <v>62</v>
       </c>
@@ -7583,7 +7585,7 @@
       <c r="H11" s="155"/>
       <c r="I11" s="155"/>
     </row>
-    <row r="12" spans="2:9" s="150" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" s="150" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="156" t="s">
         <v>63</v>
       </c>
@@ -7595,7 +7597,7 @@
       <c r="H12" s="155"/>
       <c r="I12" s="155"/>
     </row>
-    <row r="13" spans="2:9" s="150" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" s="150" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="156" t="s">
         <v>65</v>
       </c>
@@ -7607,7 +7609,7 @@
       <c r="H13" s="155"/>
       <c r="I13" s="155"/>
     </row>
-    <row r="14" spans="2:9" s="150" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" s="150" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="156" t="s">
         <v>79</v>
       </c>
@@ -7619,7 +7621,7 @@
       <c r="H14" s="155"/>
       <c r="I14" s="155"/>
     </row>
-    <row r="15" spans="2:9" s="150" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" s="150" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="312" t="s">
         <v>64</v>
       </c>
@@ -7631,7 +7633,7 @@
       <c r="H15" s="155"/>
       <c r="I15" s="155"/>
     </row>
-    <row r="16" spans="2:9" s="150" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9" s="150" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="313"/>
       <c r="C16" s="155"/>
       <c r="D16" s="155"/>
@@ -7641,7 +7643,7 @@
       <c r="H16" s="155"/>
       <c r="I16" s="155"/>
     </row>
-    <row r="17" spans="2:9" s="150" customFormat="1" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" s="150" customFormat="1" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="171" t="s">
         <v>74</v>
       </c>
@@ -7653,7 +7655,7 @@
       <c r="H17" s="151"/>
       <c r="I17" s="151"/>
     </row>
-    <row r="18" spans="2:9" s="150" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" s="150" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="168" t="s">
         <v>77</v>
       </c>
@@ -7665,7 +7667,7 @@
       <c r="H18" s="154"/>
       <c r="I18" s="154"/>
     </row>
-    <row r="19" spans="2:9" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="171" t="s">
         <v>75</v>
       </c>
@@ -7677,7 +7679,7 @@
       <c r="H19" s="154"/>
       <c r="I19" s="154"/>
     </row>
-    <row r="20" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="314" t="s">
         <v>67</v>
       </c>
@@ -7689,7 +7691,7 @@
       <c r="H20" s="150"/>
       <c r="I20" s="150"/>
     </row>
-    <row r="21" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="312"/>
       <c r="C21" s="154"/>
       <c r="D21" s="154"/>
@@ -7699,7 +7701,7 @@
       <c r="H21" s="154"/>
       <c r="I21" s="154"/>
     </row>
-    <row r="22" spans="2:9" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="313"/>
       <c r="C22" s="154"/>
       <c r="D22" s="154"/>
@@ -7709,7 +7711,7 @@
       <c r="H22" s="154"/>
       <c r="I22" s="154"/>
     </row>
-    <row r="23" spans="2:9" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="171" t="s">
         <v>76</v>
       </c>
@@ -7721,7 +7723,7 @@
       <c r="H23" s="154"/>
       <c r="I23" s="154"/>
     </row>
-    <row r="24" spans="2:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="158" t="s">
         <v>78</v>
       </c>
@@ -7733,7 +7735,7 @@
       <c r="H24" s="154"/>
       <c r="I24" s="154"/>
     </row>
-    <row r="25" spans="2:9" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="157" t="s">
         <v>68</v>
       </c>
@@ -7745,7 +7747,7 @@
       <c r="H25" s="154"/>
       <c r="I25" s="154"/>
     </row>
-    <row r="26" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="160"/>
       <c r="C26" s="154"/>
       <c r="D26" s="154"/>
@@ -7755,7 +7757,7 @@
       <c r="H26" s="154"/>
       <c r="I26" s="154"/>
     </row>
-    <row r="27" spans="2:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B27" s="169" t="s">
         <v>70</v>
       </c>
@@ -7763,7 +7765,7 @@
       <c r="D27" s="159"/>
       <c r="E27" s="159"/>
     </row>
-    <row r="28" spans="2:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="163" t="s">
         <v>69</v>
       </c>
@@ -7775,7 +7777,7 @@
       <c r="H28" s="161"/>
       <c r="I28" s="161"/>
     </row>
-    <row r="29" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="315"/>
       <c r="C29" s="315"/>
       <c r="D29" s="315"/>

</xml_diff>